<commit_message>
Set parameter values for examples
</commit_message>
<xml_diff>
--- a/examples/notebooks/data/user_friendly_config.xlsx
+++ b/examples/notebooks/data/user_friendly_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmontgomery\github\popsborder\examples\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3226467C-1E8F-4B9F-9EB2-6267440F7A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED62F65-D57E-4843-AED9-7B92860E1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF28C922-546A-4075-A167-30CB40DF9A65}"/>
   </bookViews>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAB82C6-5978-4A15-84F7-AC0E870FFFBC}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1347,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="17">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>33</v>
@@ -1381,7 +1381,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Variable packaging consignnment class, sample data, and argument for config
</commit_message>
<xml_diff>
--- a/examples/notebooks/data/user_friendly_config.xlsx
+++ b/examples/notebooks/data/user_friendly_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmontgomery\github\popsborder\examples\notebooks\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMontgomery\github\popsborder\examples\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED62F65-D57E-4843-AED9-7B92860E1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E9655E-1840-4FED-B3F4-671AFE4F87E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DF28C922-546A-4075-A167-30CB40DF9A65}"/>
+    <workbookView xWindow="34410" yWindow="3840" windowWidth="21600" windowHeight="11385" xr2:uid="{DF28C922-546A-4075-A167-30CB40DF9A65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="127">
   <si>
     <t>Consignment parameters</t>
   </si>
@@ -420,10 +420,13 @@
     <t>[0.95, 18.05]</t>
   </si>
   <si>
-    <t>"data/AQIM_sample.csv"</t>
-  </si>
-  <si>
     <t>inspection/proportion/value</t>
+  </si>
+  <si>
+    <t>variable packaging</t>
+  </si>
+  <si>
+    <t>"data/varipack_sample.csv"</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1108,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1185,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
@@ -1293,7 +1296,7 @@
         <v>88</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>89</v>
@@ -1534,7 +1537,7 @@
         <v>84</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>37</v>
@@ -1560,7 +1563,7 @@
         <v>39</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,7 +1723,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F44ADA29-5E21-48A5-B483-62CAB4A16BDB}">
           <x14:formula1>
-            <xm:f>Sheet2!$B$2:$B$3</xm:f>
+            <xm:f>Sheet2!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>B14</xm:sqref>
         </x14:dataValidation>
@@ -1741,13 +1744,13 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -1844,6 +1847,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Switch selected parameters to variable packaging consignment
</commit_message>
<xml_diff>
--- a/examples/notebooks/data/user_friendly_config.xlsx
+++ b/examples/notebooks/data/user_friendly_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMontgomery\github\popsborder\examples\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E9655E-1840-4FED-B3F4-671AFE4F87E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18C8C96-41CA-4B08-AB07-61F77A5198D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34410" yWindow="3840" windowWidth="21600" windowHeight="11385" xr2:uid="{DF28C922-546A-4075-A167-30CB40DF9A65}"/>
+    <workbookView xWindow="4230" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{DF28C922-546A-4075-A167-30CB40DF9A65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1108,7 +1108,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,7 +1282,7 @@
         <v>87</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>37</v>

</xml_diff>